<commit_message>
Updated the loc_holiday file
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/loc_holiday.xlsx
+++ b/mosip_master/xlsx/loc_holiday.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1091460\Downloads\mosip-data-1.2.0.1\mosip-data-1.2.0.1\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8EE9D8-5EBC-4B1B-A1DC-D3C7BEDEE628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D585E0-F50F-49B8-8D03-3888B259EDD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$I$1:$J$397</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -93,6 +93,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -582,12 +585,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -912,7 +916,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection sqref="A1:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -920,7 +924,7 @@
     <col min="1" max="1" width="19.1796875" customWidth="1"/>
     <col min="2" max="2" width="21.26953125" customWidth="1"/>
     <col min="3" max="3" width="22.81640625" customWidth="1"/>
-    <col min="4" max="4" width="19.1796875" customWidth="1"/>
+    <col min="4" max="4" width="19.1796875" style="3" customWidth="1"/>
     <col min="5" max="5" width="39.7265625" customWidth="1"/>
     <col min="6" max="6" width="24.81640625" customWidth="1"/>
   </cols>
@@ -935,7 +939,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -958,8 +962,8 @@
       <c r="C2">
         <v>1001</v>
       </c>
-      <c r="D2">
-        <v>44197</v>
+      <c r="D2" s="3">
+        <v>43466</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -984,8 +988,8 @@
       <c r="C3">
         <v>1001</v>
       </c>
-      <c r="D3">
-        <v>44222</v>
+      <c r="D3" s="3">
+        <v>43586</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -1009,8 +1013,8 @@
       <c r="C4">
         <v>1001</v>
       </c>
-      <c r="D4">
-        <v>44317</v>
+      <c r="D4" s="3">
+        <v>43586</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -1034,7 +1038,7 @@
       <c r="C5">
         <v>1001</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>44423</v>
       </c>
       <c r="E5" t="s">
@@ -1059,7 +1063,7 @@
       <c r="C6">
         <v>1001</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>44471</v>
       </c>
       <c r="E6" t="s">
@@ -1084,7 +1088,7 @@
       <c r="C7">
         <v>1001</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>44444</v>
       </c>
       <c r="E7" t="s">
@@ -1109,7 +1113,7 @@
       <c r="C8">
         <v>1001</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <v>44502</v>
       </c>
       <c r="E8" t="s">
@@ -1134,7 +1138,7 @@
       <c r="C9">
         <v>1001</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>44555</v>
       </c>
       <c r="E9" t="s">

</xml_diff>

<commit_message>
Updated the loc_holiday date format in the file
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/loc_holiday.xlsx
+++ b/mosip_master/xlsx/loc_holiday.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1091460\Downloads\mosip-data-1.2.0.1\mosip-data-1.2.0.1\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61993F7E-8AA9-434F-90D4-470E602178F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E618C305-5BD6-48EA-B599-FB217515F35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,6 +93,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -582,13 +585,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -921,7 +925,7 @@
     <col min="1" max="1" width="19.1796875" style="1" customWidth="1"/>
     <col min="2" max="2" width="21.26953125" style="1" customWidth="1"/>
     <col min="3" max="3" width="22.81640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.1796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.1796875" style="4" customWidth="1"/>
     <col min="5" max="5" width="39.7265625" style="1" customWidth="1"/>
     <col min="6" max="6" width="24.81640625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.453125" style="1"/>
@@ -937,7 +941,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -960,7 +964,7 @@
       <c r="C2" s="1">
         <v>1001</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="4">
         <v>43466</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -986,7 +990,7 @@
       <c r="C3" s="1">
         <v>1001</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="4">
         <v>43586</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -1011,7 +1015,7 @@
       <c r="C4" s="1">
         <v>1001</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="4">
         <v>43586</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -1036,7 +1040,7 @@
       <c r="C5" s="1">
         <v>1001</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="4">
         <v>44423</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -1061,7 +1065,7 @@
       <c r="C6" s="1">
         <v>1001</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="4">
         <v>44471</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -1086,7 +1090,7 @@
       <c r="C7" s="1">
         <v>1001</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="4">
         <v>44444</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -1111,7 +1115,7 @@
       <c r="C8" s="1">
         <v>1001</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="4">
         <v>44502</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -1136,7 +1140,7 @@
       <c r="C9" s="1">
         <v>1001</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="4">
         <v>44555</v>
       </c>
       <c r="E9" s="1" t="s">

</xml_diff>

<commit_message>
Updated the loc_holiday,registration_center and registration_center_h files
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/loc_holiday.xlsx
+++ b/mosip_master/xlsx/loc_holiday.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1091460\Downloads\mosip-data-1.2.0.1\mosip-data-1.2.0.1\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E618C305-5BD6-48EA-B599-FB217515F35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A32CA9-4B0B-4A11-B96C-165462E6B6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,9 +93,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
-  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -592,7 +589,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -917,7 +914,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>